<commit_message>
Se agrega documentacion al proyecto
</commit_message>
<xml_diff>
--- a/docs/Educción de requisitos/Requisitos funcionales.xlsx
+++ b/docs/Educción de requisitos/Requisitos funcionales.xlsx
@@ -156,7 +156,7 @@
     <t>Control interno</t>
   </si>
   <si>
-    <t>genarales</t>
+    <t>generales</t>
   </si>
 </sst>
 </file>
@@ -291,15 +291,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -309,29 +300,38 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -616,108 +616,108 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="97.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.77734375" style="1" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="11" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="9">
-        <v>43380</v>
-      </c>
-      <c r="D2" s="10"/>
+      <c r="C2" s="6">
+        <v>43352</v>
+      </c>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="12"/>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="4"/>
+      <c r="B5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="13"/>
       <c r="D5" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="4"/>
+      <c r="B7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="13"/>
       <c r="D7" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="4"/>
+      <c r="B9" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="13"/>
       <c r="D9" s="3" t="s">
         <v>43</v>
       </c>
@@ -726,66 +726,66 @@
       <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="6"/>
+      <c r="B10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="11"/>
       <c r="D10" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="14"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="6"/>
+      <c r="B12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="11"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="14"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="6"/>
+      <c r="B14" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="11"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="14"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="6"/>
+      <c r="B16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="11"/>
       <c r="D16" s="3" t="s">
         <v>43</v>
       </c>
@@ -794,20 +794,20 @@
       <c r="A17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="6"/>
+      <c r="B17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="11"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="6"/>
+      <c r="B18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="11"/>
       <c r="D18" s="3" t="s">
         <v>43</v>
       </c>
@@ -816,10 +816,10 @@
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="6"/>
+      <c r="B19" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="11"/>
       <c r="D19" s="3" t="s">
         <v>43</v>
       </c>
@@ -828,28 +828,28 @@
       <c r="A20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="6"/>
+      <c r="B20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="11"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="14"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" s="6"/>
+      <c r="B22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="11"/>
       <c r="D22" s="3" t="s">
         <v>43</v>
       </c>
@@ -858,168 +858,168 @@
       <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C23" s="6"/>
+      <c r="B23" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="11"/>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="6"/>
+      <c r="B24" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="11"/>
       <c r="D24" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="14"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="6"/>
+      <c r="B26" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="11"/>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="6"/>
+      <c r="B27" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="11"/>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="6"/>
+      <c r="B28" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="11"/>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C29" s="6"/>
+      <c r="B29" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="11"/>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="6"/>
+      <c r="B30" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="11"/>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C31" s="6"/>
+      <c r="B31" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="11"/>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C32" s="6"/>
+      <c r="B32" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="11"/>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B33" s="14"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="6"/>
+      <c r="B34" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="11"/>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="6"/>
+      <c r="B35" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="11"/>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C36" s="6"/>
+      <c r="B36" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="11"/>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="6"/>
+      <c r="B37" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="11"/>
       <c r="D37" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B38" s="14"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="16"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" s="6"/>
+      <c r="B39" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="11"/>
       <c r="D39" s="3" t="s">
         <v>43</v>
       </c>
@@ -1028,10 +1028,10 @@
       <c r="A40" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="6"/>
+      <c r="B40" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="11"/>
       <c r="D40" s="3" t="s">
         <v>43</v>
       </c>
@@ -1040,36 +1040,40 @@
       <c r="A41" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B41" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C41" s="6"/>
+      <c r="B41" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="11"/>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" s="6"/>
+      <c r="B42" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="11"/>
       <c r="D42" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B21:D21"/>
     <mergeCell ref="B25:D25"/>
     <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
@@ -1079,27 +1083,23 @@
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>